<commit_message>
Updated stress unit tests; fixed stress median calculation for even number of windows where the median is the avg between non-consecutive numbers
</commit_message>
<xml_diff>
--- a/source/activity/stress/tests/StressAlgorithmsSampleOutput.xlsx
+++ b/source/activity/stress/tests/StressAlgorithmsSampleOutput.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Meditate\source\activity\hrv\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vlado\garmin-connect-workspace\Meditate\source\activity\stress\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="11_3DC74F0148C77A779BAB0A7D334CF5B224FEA57C" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{282E41F8-8F48-44AD-9D49-7AFBF9EDC1B7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EBC" sheetId="3" r:id="rId1"/>
     <sheet name="Max-Min HR Window 10 Sec" sheetId="5" r:id="rId2"/>
     <sheet name="Max-Min HR Window 10 Sec Stats" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <definedNames>
+    <definedName name="CalculationArea">'Max-Min HR Window 10 Sec Stats'!$B$2:$B$26</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>bpm each second</t>
   </si>
@@ -67,12 +69,15 @@
   </si>
   <si>
     <t>Max-Min Window</t>
+  </si>
+  <si>
+    <t>3x Median</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -433,27 +438,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.3515625" customWidth="1"/>
-    <col min="2" max="2" width="12.23828125" customWidth="1"/>
-    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.46875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.46875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.25390625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,7 +484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>58</v>
       </c>
@@ -515,19 +520,19 @@
         <v>1034.48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B17" si="0">(60 * 1000) / A3</f>
+        <f t="shared" ref="B3:B10" si="0">(60 * 1000) / A3</f>
         <v>1000</v>
       </c>
       <c r="J3">
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>59</v>
       </c>
@@ -539,7 +544,7 @@
         <v>1016.94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>58</v>
       </c>
@@ -551,7 +556,7 @@
         <v>1034.48</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>59</v>
       </c>
@@ -563,7 +568,7 @@
         <v>1016.94</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>58</v>
       </c>
@@ -575,7 +580,7 @@
         <v>1034.48</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>58</v>
       </c>
@@ -587,7 +592,7 @@
         <v>1034.48</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>59</v>
       </c>
@@ -599,7 +604,7 @@
         <v>1016.94</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>58</v>
       </c>
@@ -611,88 +616,115 @@
         <v>1034.48</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>60</v>
       </c>
       <c r="B11">
-        <f>(60 * 1000) / A11</f>
+        <f t="shared" ref="B11:B20" si="1">(60 * 1000) / A11</f>
         <v>1000</v>
       </c>
       <c r="J11">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>60</v>
       </c>
       <c r="B12">
-        <f>(60 * 1000) / A12</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="J12">
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>59</v>
       </c>
       <c r="B13">
-        <f>(60 * 1000) / A13</f>
+        <f t="shared" si="1"/>
         <v>1016.9491525423729</v>
       </c>
       <c r="J13">
         <v>1016.94</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>59</v>
       </c>
       <c r="B14">
-        <f>(60 * 1000) / A14</f>
+        <f t="shared" si="1"/>
         <v>1016.9491525423729</v>
       </c>
       <c r="J14">
         <v>1016.94</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>57</v>
       </c>
       <c r="B15">
-        <f>(60 * 1000) / A15</f>
+        <f t="shared" si="1"/>
         <v>1052.6315789473683</v>
       </c>
       <c r="J15">
         <v>1052.6300000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>58</v>
       </c>
       <c r="B16">
-        <f>(60 * 1000) / A16</f>
+        <f t="shared" si="1"/>
         <v>1034.4827586206898</v>
       </c>
       <c r="J16">
         <v>1034.48</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>60</v>
       </c>
       <c r="B17">
-        <f>(60 * 1000) / A17</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
       <c r="J17">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>75</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>100</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>1463.4146341463415</v>
       </c>
     </row>
   </sheetData>
@@ -701,24 +733,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B579A42-728E-40A2-87FD-402B9DFD1486}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{DED22ABF-1035-5398-BCE5-6468710E342C}">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5625" customWidth="1"/>
-    <col min="3" max="3" width="14.66015625" customWidth="1"/>
-    <col min="4" max="4" width="10.22265625" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.76171875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,59 +758,49 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>58</v>
+        <v>1500</v>
       </c>
       <c r="B2">
         <f>MAX(A2:A11)-MIN(A2:A11)</f>
-        <v>12</v>
+        <v>534</v>
       </c>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>53</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -787,24 +809,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8375A381-6568-403D-B16E-684F7936B506}">
-  <dimension ref="A1:K26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{F34976B4-FE0C-5677-BE68-F6B0D0F4DDB3}">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.2265625" customWidth="1"/>
-    <col min="3" max="3" width="13.31640625" customWidth="1"/>
-    <col min="4" max="4" width="10.22265625" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.76171875" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -823,33 +845,43 @@
       <c r="F1" t="s">
         <v>12</v>
       </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
       <c r="I1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>IF(A2&lt;30, A2, 30)</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>MEDIAN(CalculationArea)</f>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF(CalculationArea, "&lt;="&amp;C2)/COUNT(CalculationArea)</f>
+        <v>0.75</v>
+      </c>
+      <c r="E2">
+        <f>COUNTIF(CalculationArea, "&gt;"&amp;C2)/COUNT(CalculationArea)-F2</f>
+        <v>0.25</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(CalculationArea, "&gt;="&amp;G2)/COUNT(CalculationArea)</f>
         <v>0</v>
       </c>
-      <c r="B2">
-        <f>IF(A2&lt;10, A2, 10)</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>MEDIAN(B2:B11)</f>
-        <v>4.5</v>
-      </c>
-      <c r="D2">
-        <f>COUNTIF(B2:B11, "&lt;="&amp;C2)/COUNT(B2:B11)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E2">
-        <f>COUNTIF(B2:B11, "&gt;"&amp;C2)/COUNT(B2:B11)-F2</f>
-        <v>0.5</v>
-      </c>
-      <c r="F2">
-        <f>COUNTIF(B2:B11, "&gt;=10")/COUNT(B2:B11)</f>
-        <v>0</v>
+      <c r="G2">
+        <f>3*C2</f>
+        <v>12</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -862,14 +894,17 @@
         <v>10</v>
       </c>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <f>IF(A3&lt;10, A3, 10)</f>
-        <v>1</v>
+        <f t="shared" ref="B3:B26" si="0">IF(A3&lt;30, A3, 30)</f>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -877,236 +912,170 @@
       <c r="I3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B3:B26" si="0">IF(A4&lt;10, A4, 10)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="M6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="H12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="H13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H14">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
       <c r="H15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="H16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="H17">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="H18">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>25</v>
       </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>8</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>